<commit_message>
Reinitialize & regen all with `make setup`
</commit_message>
<xml_diff>
--- a/project/excel/dcat_4c_ap.xlsx
+++ b/project/excel/dcat_4c_ap.xlsx
@@ -1,70 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Activity" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Agent" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Attribution" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Catalogue" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CatalogueRecord" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Checksum" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChecksumAlgorithm" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concept" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ConceptScheme" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataService" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dataset" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DatasetSeries" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Distribution" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Document" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Frequency" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Geometry" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Identifier" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kind" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LegalResource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LicenseDocument" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LinguisticSystem" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Location" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MediaType" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MediaTypeOrExtent" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PeriodOfTime" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Policy" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProvenanceStatement" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relationship" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RightsStatement" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Role" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Standard" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SupportiveEntity" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeInstant" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DefinedTerm" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NFDIDataset" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NFDICatalog" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ResearchActivity" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EntityOfInterest" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ActivityOfInterest" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tool" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Environment" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plan" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QualitativeAttribute" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantitativeAttribute" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NMRDataset" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NMRSpectroscopy" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalReaction" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSubstance" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalEntity" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSample" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HardwareTool" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SoftwareTool" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Laboratory" sheetId="54" state="visible" r:id="rId54"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="InChIKey" sheetId="55" state="visible" r:id="rId55"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="InChi" sheetId="56" state="visible" r:id="rId56"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IUPACChemicalFormula" sheetId="57" state="visible" r:id="rId57"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SMILES" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet name="Activity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Agent" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Attribution" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Catalogue" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="CatalogueRecord" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Checksum" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ChecksumAlgorithm" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Concept" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ConceptScheme" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="DataService" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Dataset" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="DatasetSeries" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Distribution" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Document" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Frequency" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Geometry" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Identifier" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Kind" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="LegalResource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="LicenseDocument" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="LinguisticSystem" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Location" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="MediaType" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="MediaTypeOrExtent" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="PeriodOfTime" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Policy" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="ProvenanceStatement" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Relationship" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Resource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="RightsStatement" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Role" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Standard" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="SupportiveEntity" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="TimeInstant" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="DefinedTerm" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="NFDIDataset" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="NFDICatalog" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="ResearchActivity" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="EntityOfInterest" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="ActivityOfInterest" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="Tool" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="Environment" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="Plan" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="QualitativeAttribute" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="QuantitativeAttribute" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="NMRDataset" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="NMRSpectroscopy" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="ChemicalReaction" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="ChemicalSubstance" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="ChemicalEntity" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="ChemicalSample" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="HardwareTool" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="SoftwareTool" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet name="Laboratory" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet name="InChIKey" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet name="InChi" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet name="IUPACChemicalFormula" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet name="SMILES" sheetId="58" state="visible" r:id="rId58"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Run `just test` & `just gen-project` to regenerate all artifacts
</commit_message>
<xml_diff>
--- a/project/excel/dcat_4c_ap.xlsx
+++ b/project/excel/dcat_4c_ap.xlsx
@@ -1,75 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Activity" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Agent" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Attribution" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Catalogue" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CatalogueRecord" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Checksum" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChecksumAlgorithm" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concept" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ConceptScheme" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataService" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dataset" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DatasetSeries" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Distribution" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Document" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Frequency" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Geometry" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Identifier" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kind" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LegalResource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LicenseDocument" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LinguisticSystem" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Location" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MediaType" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MediaTypeOrExtent" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PeriodOfTime" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Policy" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProvenanceStatement" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relationship" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RightsStatement" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Role" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Standard" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SupportiveEntity" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TimeInstant" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DefinedTerm" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ResearchDataset" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AnalysisDataset" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ResearchCatalog" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataCreatingActivity" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataAnalysis" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EvaluatedEntity" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AnalysedData" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EvaluatedActivity" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tool" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HardwareTool" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SoftwareTool" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Environment" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plan" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QualitativeAttribute" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantitativeAttribute" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NMRAnalysisDataset" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NMRSpectralAnalysis" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NMRSpectroscopy" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalReaction" sheetId="54" state="visible" r:id="rId54"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSubstance" sheetId="55" state="visible" r:id="rId55"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalEntity" sheetId="56" state="visible" r:id="rId56"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChemicalSample" sheetId="57" state="visible" r:id="rId57"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NMRSpectrum" sheetId="58" state="visible" r:id="rId58"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Laboratory" sheetId="59" state="visible" r:id="rId59"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="InChIKey" sheetId="60" state="visible" r:id="rId60"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="InChi" sheetId="61" state="visible" r:id="rId61"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IUPACChemicalFormula" sheetId="62" state="visible" r:id="rId62"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SMILES" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet name="Activity" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Agent" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Attribution" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Catalogue" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="CatalogueRecord" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Checksum" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ChecksumAlgorithm" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Concept" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ConceptScheme" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="DataService" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Dataset" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="DatasetSeries" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Distribution" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Document" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Frequency" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Geometry" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Identifier" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Kind" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="LegalResource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="LicenseDocument" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="LinguisticSystem" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Location" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="MediaType" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="MediaTypeOrExtent" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="PeriodOfTime" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Policy" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="ProvenanceStatement" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Relationship" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Resource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="RightsStatement" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Role" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Standard" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="SupportiveEntity" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="TimeInstant" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="DefinedTerm" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="ResearchDataset" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="AnalysisDataset" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="ResearchCatalog" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="DataCreatingActivity" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="DataAnalysis" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="EvaluatedEntity" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AnalysisSourceData" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="EvaluatedActivity" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="Tool" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="HardwareTool" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="SoftwareTool" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="Environment" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="Plan" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="QualitativeAttribute" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="QuantitativeAttribute" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="NMRAnalysisDataset" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="NMRSpectralAnalysis" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="NMRSpectroscopy" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet name="ChemicalReaction" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet name="ChemicalSubstance" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet name="ChemicalEntity" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet name="ChemicalSample" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet name="NMRSpectrum" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet name="Laboratory" sheetId="59" state="visible" r:id="rId59"/>
+    <sheet name="InChIKey" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet name="InChi" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet name="IUPACChemicalFormula" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet name="SMILES" sheetId="63" state="visible" r:id="rId63"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Regen all schema artefact and test examples
</commit_message>
<xml_diff>
--- a/project/excel/dcat_4c_ap.xlsx
+++ b/project/excel/dcat_4c_ap.xlsx
@@ -6182,192 +6182,474 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>used_pulse_sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>used_number_of_scans</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>probes_nucleus</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>used_calibration_compound</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>used_reference_compound</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>evaluated_entity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>evaluated_activity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>realized_plan</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>occurred_in</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>other_identifier</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>had_input_entity</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>had_output_entity</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>had_input_activity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>carried_out_by</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_proton_frequency</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>used_pulse_sequence</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>probes_nucleus</t>
+          <t>other_identifier</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>used_calibration_compound</t>
+          <t>has_qualitative_attribute</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>used_reference_compound</t>
+          <t>has_quantitative_attribute</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>evaluated_entity</t>
+          <t>has_part</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>evaluated_activity</t>
+          <t>type</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>realized_plan</t>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_shift_reference</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>inchi</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>inchikey</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>smiles</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>molecular_formula</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>iupac_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_molar_mass</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alternative_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_physical_state</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_temperature</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>occurred_in</t>
+          <t>has_mass</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
+          <t>has_volume</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>has_density</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>has_pressure</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>other_identifier</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_shift_reference</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>inchi</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>inchikey</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>smiles</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>molecular_formula</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>iupac_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_molar_mass</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alternative_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_physical_state</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_temperature</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_mass</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_volume</t>
+        </is>
+      </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>has_density</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>has_pressure</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>other_identifier</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_part</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>had_input_entity</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>had_output_entity</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>had_input_activity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>carried_out_by</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>has_quantitative_attribute</t>
+          <t>type</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
           <t>rdf_type</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_proton_frequency</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+  <dataValidations count="1">
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6503,63 +6785,550 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:W1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_shift_reference</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>inchi</t>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nucleus_of</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>inchikey</t>
+          <t>title</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>smiles</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>molecular_formula</t>
+          <t>other_identifier</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>iupac_name</t>
+          <t>has_qualitative_attribute</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>has_molar_mass</t>
+          <t>has_quantitative_attribute</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_percentage_of_total</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_concentration</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_ph_value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>composed_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_molar_equivalent</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_amount</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>alternative_label</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_physical_state</t>
+        </is>
+      </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>has_temperature</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_mass</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_volume</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_density</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>has_pressure</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>other_identifier</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>application_profile</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>change_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>listing_date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>modification_date</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>primary_topic</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>source_metadata</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_concentration</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_ph_value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>composed_of</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_molar_equivalent</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_amount</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_percentage_of_total</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>derived_from</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alternative_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>has_physical_state</t>
         </is>
       </c>
@@ -6590,45 +7359,50 @@
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>was_generated_by</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>title</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>other_identifier</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>has_qualitative_attribute</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>has_quantitative_attribute</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>has_part</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>rdf_type</t>
         </is>
@@ -6644,630 +7418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>inchi</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>inchikey</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>smiles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>molecular_formula</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>iupac_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_molar_mass</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nucleus_of</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_percentage_of_total</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_concentration</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_ph_value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>composed_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_molar_equivalent</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_amount</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>application_profile</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>change_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>listing_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>modification_date</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>primary_topic</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>source_metadata</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7413,189 +7564,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_concentration</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_ph_value</t>
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>composed_of</t>
+          <t>type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>has_molar_equivalent</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_amount</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_percentage_of_total</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>derived_from</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
           <t>rdf_type</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust prefixes to avoid error
</commit_message>
<xml_diff>
--- a/project/excel/dcat_4c_ap.xlsx
+++ b/project/excel/dcat_4c_ap.xlsx
@@ -57,53 +57,37 @@
     <sheet name="SupportiveEntity" sheetId="48" state="visible" r:id="rId48"/>
     <sheet name="Surrounding" sheetId="49" state="visible" r:id="rId49"/>
     <sheet name="TimeInstant" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet name="ChemicalEntity" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet name="Atom" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet name="MolarMass" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet name="InChIKey" sheetId="54" state="visible" r:id="rId54"/>
-    <sheet name="InChi" sheetId="55" state="visible" r:id="rId55"/>
-    <sheet name="MolecularFormula" sheetId="56" state="visible" r:id="rId56"/>
-    <sheet name="IUPACName" sheetId="57" state="visible" r:id="rId57"/>
-    <sheet name="SMILES" sheetId="58" state="visible" r:id="rId58"/>
-    <sheet name="Concentration" sheetId="59" state="visible" r:id="rId59"/>
-    <sheet name="AmountOfSubstance" sheetId="60" state="visible" r:id="rId60"/>
-    <sheet name="PHValue" sheetId="61" state="visible" r:id="rId61"/>
-    <sheet name="ChemicalReaction" sheetId="62" state="visible" r:id="rId62"/>
-    <sheet name="StartingMaterial" sheetId="63" state="visible" r:id="rId63"/>
-    <sheet name="DissolvingSubstance" sheetId="64" state="visible" r:id="rId64"/>
-    <sheet name="Reagent" sheetId="65" state="visible" r:id="rId65"/>
-    <sheet name="ChemicalProduct" sheetId="66" state="visible" r:id="rId66"/>
-    <sheet name="Catalyst" sheetId="67" state="visible" r:id="rId67"/>
-    <sheet name="Reactor" sheetId="68" state="visible" r:id="rId68"/>
-    <sheet name="Yield" sheetId="69" state="visible" r:id="rId69"/>
-    <sheet name="MolarEquivalent" sheetId="70" state="visible" r:id="rId70"/>
-    <sheet name="PercentageOfTotal" sheetId="71" state="visible" r:id="rId71"/>
-    <sheet name="MaterialEntity" sheetId="72" state="visible" r:id="rId72"/>
-    <sheet name="MaterialSample" sheetId="73" state="visible" r:id="rId73"/>
-    <sheet name="Temperature" sheetId="74" state="visible" r:id="rId74"/>
-    <sheet name="Mass" sheetId="75" state="visible" r:id="rId75"/>
-    <sheet name="Volume" sheetId="76" state="visible" r:id="rId76"/>
-    <sheet name="Density" sheetId="77" state="visible" r:id="rId77"/>
-    <sheet name="Pressure" sheetId="78" state="visible" r:id="rId78"/>
-    <sheet name="NMRSample" sheetId="79" state="visible" r:id="rId79"/>
-    <sheet name="NMRSampleTemperature" sheetId="80" state="visible" r:id="rId80"/>
-    <sheet name="NMRAnalysisDataset" sheetId="81" state="visible" r:id="rId81"/>
-    <sheet name="NMRSpectralAnalysis" sheetId="82" state="visible" r:id="rId82"/>
-    <sheet name="NMRSpectrum" sheetId="83" state="visible" r:id="rId83"/>
-    <sheet name="NMRSpectroscopy" sheetId="84" state="visible" r:id="rId84"/>
-    <sheet name="NMRSpectrometer" sheetId="85" state="visible" r:id="rId85"/>
-    <sheet name="ShiftCalibrationCompound" sheetId="86" state="visible" r:id="rId86"/>
-    <sheet name="ShiftReferenceCompound" sheetId="87" state="visible" r:id="rId87"/>
-    <sheet name="CharacterizedCompound" sheetId="88" state="visible" r:id="rId88"/>
-    <sheet name="AcquisitionNucleus" sheetId="89" state="visible" r:id="rId89"/>
-    <sheet name="NMRSolvent" sheetId="90" state="visible" r:id="rId90"/>
-    <sheet name="PulseSequence" sheetId="91" state="visible" r:id="rId91"/>
-    <sheet name="NominalProtonFrequency" sheetId="92" state="visible" r:id="rId92"/>
-    <sheet name="CalibrationPeakShift" sheetId="93" state="visible" r:id="rId93"/>
-    <sheet name="NumberOfScans" sheetId="94" state="visible" r:id="rId94"/>
-    <sheet name="SubstanceSample" sheetId="95" state="visible" r:id="rId95"/>
-    <sheet name="PolymerSample" sheetId="96" state="visible" r:id="rId96"/>
-    <sheet name="Laboratory" sheetId="97" state="visible" r:id="rId97"/>
+    <sheet name="MaterialEntity" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="MaterialSample" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="Temperature" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet name="Mass" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet name="Volume" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet name="Density" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet name="Pressure" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet name="ChemicalEntity" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet name="Atom" sheetId="59" state="visible" r:id="rId59"/>
+    <sheet name="MolarMass" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet name="InChIKey" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet name="InChi" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet name="MolecularFormula" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet name="IUPACName" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet name="SMILES" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet name="Concentration" sheetId="66" state="visible" r:id="rId66"/>
+    <sheet name="AmountOfSubstance" sheetId="67" state="visible" r:id="rId67"/>
+    <sheet name="PHValue" sheetId="68" state="visible" r:id="rId68"/>
+    <sheet name="ChemicalReaction" sheetId="69" state="visible" r:id="rId69"/>
+    <sheet name="StartingMaterial" sheetId="70" state="visible" r:id="rId70"/>
+    <sheet name="DissolvingSubstance" sheetId="71" state="visible" r:id="rId71"/>
+    <sheet name="Reagent" sheetId="72" state="visible" r:id="rId72"/>
+    <sheet name="ChemicalProduct" sheetId="73" state="visible" r:id="rId73"/>
+    <sheet name="Catalyst" sheetId="74" state="visible" r:id="rId74"/>
+    <sheet name="Reactor" sheetId="75" state="visible" r:id="rId75"/>
+    <sheet name="Yield" sheetId="76" state="visible" r:id="rId76"/>
+    <sheet name="MolarEquivalent" sheetId="77" state="visible" r:id="rId77"/>
+    <sheet name="PercentageOfTotal" sheetId="78" state="visible" r:id="rId78"/>
+    <sheet name="SubstanceSample" sheetId="79" state="visible" r:id="rId79"/>
+    <sheet name="PolymerSample" sheetId="80" state="visible" r:id="rId80"/>
+    <sheet name="Laboratory" sheetId="81" state="visible" r:id="rId81"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3167,6 +3151,518 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alternative_label</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_physical_state</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_temperature</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_mass</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_volume</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_density</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_pressure</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>other_identifier</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>part_of</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>derived_from</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternative_label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_physical_state</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_temperature</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_mass</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_volume</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_density</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_pressure</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>was_generated_by</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>other_identifier</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>part_of</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3302,7 +3798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3443,7 +3939,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3499,7 +4026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3545,7 +4072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3591,7 +4118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3637,7 +4164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3683,7 +4210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3729,7 +4256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3785,7 +4312,270 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_quantity_type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>used_starting_material</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>used_reactant</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>generated_product</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>used_catalyst</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>used_solvent</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_duration</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>used_reactor</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_temperature</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_pressure</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_yield</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_reaction_step</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>related_resource</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>other_identifier</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>had_input_entity</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>had_output_entity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>had_input_activity</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>carried_out_by</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>part_of</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3816,270 +4606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Z1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>used_starting_material</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>used_reactant</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>generated_product</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>used_catalyst</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>used_solvent</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_duration</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>used_reactor</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_yield</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_reaction_step</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>related_resource</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>had_input_entity</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>had_output_entity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>had_input_activity</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>carried_out_by</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4220,7 +4747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4361,7 +4888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4502,7 +5029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4643,7 +5170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4784,7 +5311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4895,549 +5422,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>derived_from</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -5879,817 +5863,136 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
+  <dimension ref="A1:Y1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_concentration</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_ph_value</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>composed_of</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>has_quantity_type</t>
+          <t>has_molar_equivalent</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>has_amount</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>has_percentage_of_total</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>derived_from</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>alternative_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_physical_state</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_temperature</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_mass</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_volume</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>has_density</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>has_pressure</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>was_generated_by</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>other_identifier</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_qualitative_attribute</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_quantitative_attribute</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>has_part</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>part_of</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
           <t>type</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AM1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>access_rights</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>applicable_legislation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>conforms_to</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>contact_point</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>creator</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>dataset_distribution</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>documentation</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>frequency</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>geographical_coverage</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_version</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>in_series</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>is_referenced_by</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>landing_page</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>modification_date</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>provenance</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>publisher</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>qualified_attribution</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>qualified_relation</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>related_resource</t>
-        </is>
-      </c>
       <c r="Y1" t="inlineStr">
-        <is>
-          <t>release_date</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>spatial_resolution</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>temporal_coverage</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>temporal_resolution</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>theme</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>version_notes</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>is_about_entity</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>is_about_activity</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:R1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>evaluated_entity</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>evaluated_activity</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>realized_plan</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>occurred_in</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>had_input_entity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>had_output_entity</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>had_input_activity</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>carried_out_by</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Z1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>used_spectrometer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>used_solvent</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>used_pulse_sequence</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>used_number_of_scans</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>used_sample_temperature</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>probes_nucleus</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>used_calibration_compound</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>used_reference_compound</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>evaluated_entity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>evaluated_activity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>realized_plan</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>occurred_in</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>had_input_entity</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>had_output_entity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>had_input_activity</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>carried_out_by</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_proton_frequency</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_calibration_shift</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>inchi</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>inchikey</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>smiles</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>molecular_formula</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>iupac_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_molar_mass</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
         <is>
           <t>rdf_type</t>
         </is>
@@ -6705,1125 +6008,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_calibration_shift</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>inchi</t>
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>inchikey</t>
+          <t>type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>smiles</t>
+          <t>rdf_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>application_profile</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>change_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>language</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>molecular_formula</t>
+          <t>listing_date</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>iupac_name</t>
+          <t>modification_date</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>has_molar_mass</t>
+          <t>primary_topic</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>alternative_label</t>
+          <t>source_metadata</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:W1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>inchi</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>inchikey</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>smiles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>molecular_formula</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>iupac_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_molar_mass</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nucleus_of</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>application_profile</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>change_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>listing_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>modification_date</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>primary_topic</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>source_metadata</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:W1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_percentage_of_total</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_concentration</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_ph_value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>composed_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_molar_equivalent</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_amount</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_quantity_type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Y1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_concentration</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_ph_value</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>composed_of</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_molar_equivalent</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_amount</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_percentage_of_total</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>derived_from</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Y1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_concentration</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_ph_value</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>composed_of</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_molar_equivalent</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_amount</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_percentage_of_total</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>derived_from</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>alternative_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>has_physical_state</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_temperature</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_mass</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_volume</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>has_density</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>has_pressure</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>was_generated_by</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>other_identifier</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>has_qualitative_attribute</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>has_quantitative_attribute</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>has_part</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>part_of</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"SOLID,CRYSTAL,LIQUID,GASEOUS"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rdf_type</t>
+          <t>title</t>
         </is>
       </c>
     </row>

</xml_diff>